<commit_message>
addtional column "project name"
addtional column "project name"
</commit_message>
<xml_diff>
--- a/employee info.xlsx
+++ b/employee info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>LAST NAME</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>WTI VIS-MIN BRANCH</t>
+  </si>
+  <si>
+    <t>PROJECT NAME</t>
   </si>
 </sst>
 </file>
@@ -285,9 +288,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -300,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -327,13 +328,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,23 +635,24 @@
     <col min="7" max="7" width="32.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" style="9" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="6"/>
+    <col min="10" max="10" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-    </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
@@ -666,12 +671,15 @@
       <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="13"/>
+      <c r="J5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="4" t="s">
         <v>6</v>
@@ -690,9 +698,10 @@
         <v>10</v>
       </c>
       <c r="H6" s="5"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="11"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
@@ -713,11 +722,12 @@
       <c r="H7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="4" t="s">
         <v>6</v>
@@ -736,9 +746,10 @@
         <v>26</v>
       </c>
       <c r="H8" s="5"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="11"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="4" t="s">
         <v>14</v>
@@ -759,11 +770,12 @@
       <c r="H9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="4" t="s">
         <v>19</v>
@@ -778,9 +790,10 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="11"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="4" t="s">
         <v>22</v>
@@ -799,11 +812,12 @@
       <c r="H11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="4" t="s">
         <v>38</v>
@@ -822,9 +836,10 @@
         <v>42</v>
       </c>
       <c r="H12" s="5"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="11"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="4" t="s">
         <v>44</v>
@@ -841,9 +856,10 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="11"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="4" t="s">
         <v>46</v>
@@ -862,9 +878,10 @@
         <v>43</v>
       </c>
       <c r="H14" s="5"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="11"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="4" t="s">
         <v>51</v>
@@ -881,9 +898,10 @@
         <v>50</v>
       </c>
       <c r="H15" s="5"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="11"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="4" t="s">
         <v>53</v>
@@ -902,7 +920,11 @@
         <v>56</v>
       </c>
       <c r="H16" s="5"/>
-      <c r="I16" s="4"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
project name enter data
project name enter data
</commit_message>
<xml_diff>
--- a/employee info.xlsx
+++ b/employee info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>LAST NAME</t>
   </si>
@@ -201,6 +201,24 @@
   </si>
   <si>
     <t>WTI VIS-MIN BRANCH</t>
+  </si>
+  <si>
+    <t>job description</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>wd</t>
+  </si>
+  <si>
+    <t>dsada</t>
   </si>
 </sst>
 </file>
@@ -327,13 +345,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,20 +652,20 @@
     <col min="10" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-    </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
@@ -666,12 +684,15 @@
       <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="12"/>
+      <c r="J5" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="4" t="s">
         <v>6</v>
@@ -691,8 +712,11 @@
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
@@ -716,8 +740,11 @@
       <c r="I7" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="4" t="s">
         <v>6</v>
@@ -737,8 +764,11 @@
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="4" t="s">
         <v>14</v>
@@ -762,8 +792,11 @@
       <c r="I9" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="4" t="s">
         <v>19</v>
@@ -779,8 +812,11 @@
       <c r="G10" s="4"/>
       <c r="H10" s="5"/>
       <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="4" t="s">
         <v>22</v>
@@ -802,8 +838,11 @@
       <c r="I11" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="4" t="s">
         <v>38</v>
@@ -823,8 +862,11 @@
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="4" t="s">
         <v>44</v>
@@ -843,7 +885,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="4" t="s">
         <v>46</v>
@@ -864,7 +906,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="4" t="s">
         <v>51</v>
@@ -883,7 +925,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="4" t="s">
         <v>53</v>

</xml_diff>